<commit_message>
Evaluation Implementations - Progress Save
</commit_message>
<xml_diff>
--- a/Results/Training_Plan.xlsx
+++ b/Results/Training_Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96b2e28e11ffcb6a/Dokumente/Studium-Vincents-Surface/Master/Unterlagen/Master Thesis/Repository/MasterThesis/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="11_AD4DB114E441178AC67DF4162E17CDD6683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A988C93B-D422-43EC-999F-9BFBFEEFED1B}"/>
+  <xr:revisionPtr revIDLastSave="293" documentId="11_AD4DB114E441178AC67DF4162E17CDD6683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C5C7660-1FC6-40D4-9865-E0302D5117ED}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="43">
   <si>
     <t>Input Columns</t>
   </si>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1120,6 +1120,24 @@
       <c r="F10" s="29" t="s">
         <v>40</v>
       </c>
+      <c r="G10" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="27" t="s">
+        <v>20</v>
+      </c>
       <c r="M10" s="28" t="s">
         <v>30</v>
       </c>
@@ -1146,6 +1164,24 @@
       <c r="F11" s="29" t="s">
         <v>40</v>
       </c>
+      <c r="G11" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="27" t="s">
+        <v>20</v>
+      </c>
       <c r="M11" s="28" t="s">
         <v>30</v>
       </c>
@@ -1172,6 +1208,24 @@
       <c r="F12" s="29" t="s">
         <v>40</v>
       </c>
+      <c r="G12" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="27" t="s">
+        <v>20</v>
+      </c>
       <c r="M12" s="28" t="s">
         <v>31</v>
       </c>
@@ -1200,6 +1254,24 @@
       <c r="F13" s="29" t="s">
         <v>40</v>
       </c>
+      <c r="G13" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="27" t="s">
+        <v>20</v>
+      </c>
       <c r="M13" s="28" t="s">
         <v>31</v>
       </c>
@@ -1303,6 +1375,24 @@
       <c r="F16" s="29" t="s">
         <v>40</v>
       </c>
+      <c r="G16" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="27" t="s">
+        <v>20</v>
+      </c>
       <c r="M16" s="28" t="s">
         <v>34</v>
       </c>
@@ -1326,6 +1416,24 @@
       <c r="F17" s="29" t="s">
         <v>40</v>
       </c>
+      <c r="G17" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="27" t="s">
+        <v>20</v>
+      </c>
       <c r="M17" s="28" t="s">
         <v>34</v>
       </c>
@@ -1355,6 +1463,24 @@
       <c r="F18" s="29" t="s">
         <v>40</v>
       </c>
+      <c r="G18" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="27" t="s">
+        <v>20</v>
+      </c>
       <c r="M18" s="28" t="s">
         <v>35</v>
       </c>
@@ -1383,6 +1509,24 @@
       </c>
       <c r="F19" s="29" t="s">
         <v>40</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="27" t="s">
+        <v>20</v>
       </c>
       <c r="M19" s="28" t="s">
         <v>35</v>

</xml_diff>